<commit_message>
Update Digital Playbook Mapping
</commit_message>
<xml_diff>
--- a/artifacts/Digital Playbook Mapping.xlsx
+++ b/artifacts/Digital Playbook Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdamashek\SharePoint\ODEA - Documents\GSA 18F\Pool 2 docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdamashek\Documents\GitHub\OpenFDA\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,57 @@
   </si>
   <si>
     <t>ODEA Phase</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDA/blob/master/artifacts/Discovery%20and%20Requirements%20Analysis.docx</t>
+  </si>
+  <si>
+    <t>Review mapping of Epic 1 user stories to API data</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDA/blob/master/Artifacts/Design%20Delivery.docx</t>
+  </si>
+  <si>
+    <t>Select Epic 1 user stories for Sprint Backlog</t>
+  </si>
+  <si>
+    <t>https://github.com/binarygroup/OpenFDA/blob/master/artifacts/Skype%20Discussion%20Thread.docx</t>
+  </si>
+  <si>
+    <t>Setup Ruby on Rails environment</t>
+  </si>
+  <si>
+    <t>Assess using Kibana as extension of FDA elasticsearch</t>
+  </si>
+  <si>
+    <t>Setup GitHub for team</t>
+  </si>
+  <si>
+    <t>Leverage Kibana source as a reference and build on AngularJS</t>
+  </si>
+  <si>
+    <t>Review Product Backlog</t>
+  </si>
+  <si>
+    <t>Setup AWS Elastic Beanstalk instance</t>
+  </si>
+  <si>
+    <t>Review Design Prototype v1</t>
+  </si>
+  <si>
+    <t>Arrange for user SME acceptance at Sprint Review</t>
+  </si>
+  <si>
+    <t>Select Continuous Integration tool and leverage Elastic Beanstalk CM capabilities</t>
+  </si>
+  <si>
+    <t>Review Development Prototype changes</t>
+  </si>
+  <si>
+    <t>Review and accept Development Prototype</t>
   </si>
 </sst>
 </file>
@@ -224,7 +275,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +287,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -258,10 +317,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -281,8 +341,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -564,10 +626,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16:S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,6 +704,586 @@
         <v>58</v>
       </c>
     </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>42175</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>42176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>42176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>42176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>42175</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="I6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>42176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>42176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>42177</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>42179</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>42179</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>42180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>42184</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>42187</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>42191</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>42192</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
@@ -657,8 +1299,14 @@
       <formula1>Pools</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -670,7 +1318,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,18 +1675,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1061,14 +1709,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDF1648-5EF8-4D8D-B906-BEFEFDAED3B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1083,4 +1723,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEF8AAF-20F9-4AFF-B5F6-D38EF6D62C46}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>